<commit_message>
Shuffled SO 1215 and PredictionSet3
</commit_message>
<xml_diff>
--- a/PredictionSet.xlsx
+++ b/PredictionSet.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Farshad\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Farshad\Desktop\Git repos\Structural_Engineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79728AB-1C1A-4E1C-A1CF-B943100E6D9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6226AD22-798E-441C-946A-BC0BCC4C97B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="330" yWindow="255" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -381,7 +381,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,16 +444,16 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>0.47421799999999997</v>
+        <v>47.421799999999998</v>
       </c>
       <c r="I2">
-        <v>0.42405300000000001</v>
+        <v>42.405300000000004</v>
       </c>
       <c r="J2">
-        <v>7.7089000000000005E-2</v>
+        <v>7.7089000000000008</v>
       </c>
       <c r="K2">
-        <v>4.7625000000000001E-2</v>
+        <v>4.7625000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -479,16 +479,16 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0.49784</v>
+        <v>49.783999999999999</v>
       </c>
       <c r="I3">
-        <v>0.43205399999999999</v>
+        <v>43.205399999999997</v>
       </c>
       <c r="J3">
-        <v>8.8900000000000007E-2</v>
+        <v>8.89</v>
       </c>
       <c r="K3">
-        <v>5.5626000000000002E-2</v>
+        <v>5.5625999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -514,16 +514,16 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <v>0.53136799999999995</v>
+        <v>53.136799999999994</v>
       </c>
       <c r="I4">
-        <v>0.44234099999999998</v>
+        <v>44.234099999999998</v>
       </c>
       <c r="J4">
-        <v>0.10566399999999999</v>
+        <v>10.5664</v>
       </c>
       <c r="K4">
-        <v>6.5912999999999999E-2</v>
+        <v>6.5913000000000004</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -549,16 +549,16 @@
         <v>1</v>
       </c>
       <c r="H5">
-        <v>0.53136799999999995</v>
+        <v>53.136799999999994</v>
       </c>
       <c r="I5">
-        <v>0.44234099999999998</v>
+        <v>44.234099999999998</v>
       </c>
       <c r="J5">
-        <v>0.10566399999999999</v>
+        <v>10.5664</v>
       </c>
       <c r="K5">
-        <v>6.5912999999999999E-2</v>
+        <v>6.5913000000000004</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -584,16 +584,16 @@
         <v>1</v>
       </c>
       <c r="H6">
-        <v>1.066038</v>
+        <v>106.60380000000001</v>
       </c>
       <c r="I6">
-        <v>0.45694600000000002</v>
+        <v>45.694600000000001</v>
       </c>
       <c r="J6">
-        <v>0.10896599999999999</v>
+        <v>10.896599999999999</v>
       </c>
       <c r="K6">
-        <v>6.0451999999999999E-2</v>
+        <v>6.0451999999999995</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -619,16 +619,16 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0.53136799999999995</v>
+        <v>53.136799999999994</v>
       </c>
       <c r="I7">
-        <v>0.44234099999999998</v>
+        <v>44.234099999999998</v>
       </c>
       <c r="J7">
-        <v>0.10566399999999999</v>
+        <v>10.5664</v>
       </c>
       <c r="K7">
-        <v>6.5912999999999999E-2</v>
+        <v>6.5913000000000004</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -654,16 +654,16 @@
         <v>1</v>
       </c>
       <c r="H8">
-        <v>0.99212400000000001</v>
+        <v>99.212400000000002</v>
       </c>
       <c r="I8">
-        <v>0.44983400000000001</v>
+        <v>44.983400000000003</v>
       </c>
       <c r="J8">
-        <v>3.2003999999999998E-2</v>
+        <v>3.2003999999999997</v>
       </c>
       <c r="K8">
-        <v>1.8034000000000001E-2</v>
+        <v>1.8034000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>